<commit_message>
Minor cosmetics in altfun sheet.
</commit_message>
<xml_diff>
--- a/altfun/stm32f051.xlsx
+++ b/altfun/stm32f051.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marten\Code\stm32f0\altfun\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marten\Code\hal\altfun\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE9B54C9-6BEB-4051-855F-2174164D5515}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C05664FE-336A-4AC8-A676-7A301B068A28}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1905" yWindow="45" windowWidth="27945" windowHeight="20775" xr2:uid="{32DCDEAA-12F8-4952-BE27-29A2D20BACB4}"/>
+    <workbookView xWindow="-36840" yWindow="60" windowWidth="27945" windowHeight="20775" xr2:uid="{32DCDEAA-12F8-4952-BE27-29A2D20BACB4}"/>
   </bookViews>
   <sheets>
     <sheet name="stm32f051" sheetId="1" r:id="rId1"/>
@@ -938,7 +938,6 @@
     </font>
     <font>
       <b/>
-      <u/>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -953,12 +952,21 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -1003,10 +1011,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1326,7 +1334,7 @@
   <dimension ref="B3:M77"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>